<commit_message>
Added pin assignment for AksIM
</commit_message>
<xml_diff>
--- a/hardware/pins.xlsx
+++ b/hardware/pins.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="104">
   <si>
     <t xml:space="preserve">All pins are 3.3V logic</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">gpio0[13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AksIM</t>
   </si>
   <si>
     <t xml:space="preserve">gpio1[31]</t>
@@ -343,6 +346,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -364,12 +368,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,7 +487,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,17 +591,17 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,6 +685,7 @@
       <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="0"/>
       <c r="E6" s="9"/>
       <c r="G6" s="14" t="n">
         <v>1</v>
@@ -696,6 +703,7 @@
       <c r="B7" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="0"/>
       <c r="E7" s="9"/>
       <c r="G7" s="14" t="n">
         <v>2</v>
@@ -844,6 +852,7 @@
       <c r="A14" s="14" t="n">
         <v>9</v>
       </c>
+      <c r="C14" s="0"/>
       <c r="D14" s="0" t="s">
         <v>23</v>
       </c>
@@ -936,6 +945,7 @@
       <c r="A18" s="14" t="n">
         <v>13</v>
       </c>
+      <c r="C18" s="0"/>
       <c r="D18" s="0" t="s">
         <v>34</v>
       </c>
@@ -1090,6 +1100,7 @@
       <c r="A24" s="14" t="n">
         <v>19</v>
       </c>
+      <c r="C24" s="0"/>
       <c r="D24" s="0" t="s">
         <v>54</v>
       </c>
@@ -1097,11 +1108,18 @@
       <c r="G24" s="14" t="n">
         <v>19</v>
       </c>
-      <c r="I24" s="1"/>
+      <c r="H24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>7</v>
+      </c>
       <c r="J24" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="9"/>
+      <c r="K24" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="n">
@@ -1110,7 +1128,7 @@
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
       <c r="D25" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>11</v>
@@ -1120,7 +1138,7 @@
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K25" s="9"/>
     </row>
@@ -1131,7 +1149,7 @@
       <c r="B26" s="16"/>
       <c r="C26" s="17"/>
       <c r="D26" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>11</v>
@@ -1140,13 +1158,13 @@
         <v>21</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>49</v>
@@ -1159,7 +1177,7 @@
       <c r="B27" s="16"/>
       <c r="C27" s="17"/>
       <c r="D27" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>11</v>
@@ -1168,13 +1186,13 @@
         <v>22</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>49</v>
@@ -1187,7 +1205,7 @@
       <c r="B28" s="16"/>
       <c r="C28" s="17"/>
       <c r="D28" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>11</v>
@@ -1197,7 +1215,7 @@
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K28" s="9"/>
     </row>
@@ -1208,7 +1226,7 @@
       <c r="B29" s="16"/>
       <c r="C29" s="17"/>
       <c r="D29" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>11</v>
@@ -1218,7 +1236,7 @@
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K29" s="9"/>
     </row>
@@ -1229,7 +1247,7 @@
       <c r="B30" s="16"/>
       <c r="C30" s="17"/>
       <c r="D30" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>11</v>
@@ -1239,7 +1257,7 @@
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K30" s="9"/>
     </row>
@@ -1247,8 +1265,9 @@
       <c r="A31" s="14" t="n">
         <v>26</v>
       </c>
+      <c r="C31" s="0"/>
       <c r="D31" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E31" s="9"/>
       <c r="G31" s="14" t="n">
@@ -1256,7 +1275,7 @@
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K31" s="9"/>
     </row>
@@ -1267,17 +1286,17 @@
       <c r="B32" s="16"/>
       <c r="C32" s="17"/>
       <c r="D32" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G32" s="14" t="n">
         <v>27</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K32" s="9"/>
     </row>
@@ -1288,25 +1307,25 @@
       <c r="B33" s="16"/>
       <c r="C33" s="17"/>
       <c r="D33" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G33" s="14" t="n">
         <v>28</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,22 +1335,22 @@
       <c r="B34" s="16"/>
       <c r="C34" s="17"/>
       <c r="D34" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G34" s="14" t="n">
         <v>29</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K34" s="9"/>
     </row>
@@ -1342,25 +1361,25 @@
       <c r="B35" s="16"/>
       <c r="C35" s="17"/>
       <c r="D35" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G35" s="14" t="n">
         <v>30</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I35" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,25 +1389,25 @@
       <c r="B36" s="16"/>
       <c r="C36" s="17"/>
       <c r="D36" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G36" s="14" t="n">
         <v>31</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,10 +1417,10 @@
       <c r="B37" s="16"/>
       <c r="C37" s="17"/>
       <c r="D37" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G37" s="14" t="n">
         <v>32</v>
@@ -1416,10 +1435,10 @@
       <c r="B38" s="16"/>
       <c r="C38" s="17"/>
       <c r="D38" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G38" s="14" t="n">
         <v>33</v>
@@ -1434,10 +1453,10 @@
       <c r="B39" s="16"/>
       <c r="C39" s="17"/>
       <c r="D39" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G39" s="14" t="n">
         <v>34</v>
@@ -1452,10 +1471,10 @@
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
       <c r="D40" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G40" s="14" t="n">
         <v>35</v>
@@ -1470,10 +1489,10 @@
       <c r="B41" s="16"/>
       <c r="C41" s="17"/>
       <c r="D41" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G41" s="14" t="n">
         <v>36</v>
@@ -1488,10 +1507,10 @@
       <c r="B42" s="16"/>
       <c r="C42" s="17"/>
       <c r="D42" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G42" s="14" t="n">
         <v>37</v>
@@ -1506,10 +1525,10 @@
       <c r="B43" s="16"/>
       <c r="C43" s="17"/>
       <c r="D43" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G43" s="14" t="n">
         <v>38</v>
@@ -1524,10 +1543,10 @@
       <c r="B44" s="16"/>
       <c r="C44" s="17"/>
       <c r="D44" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G44" s="14" t="n">
         <v>39</v>
@@ -1542,10 +1561,10 @@
       <c r="B45" s="16"/>
       <c r="C45" s="17"/>
       <c r="D45" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G45" s="14" t="n">
         <v>40</v>
@@ -1560,10 +1579,10 @@
       <c r="B46" s="16"/>
       <c r="C46" s="17"/>
       <c r="D46" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G46" s="14" t="n">
         <v>41</v>
@@ -1578,10 +1597,10 @@
       <c r="B47" s="16"/>
       <c r="C47" s="17"/>
       <c r="D47" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G47" s="14" t="n">
         <v>42</v>
@@ -1596,10 +1615,10 @@
       <c r="B48" s="16"/>
       <c r="C48" s="17"/>
       <c r="D48" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G48" s="14" t="n">
         <v>43</v>
@@ -1617,10 +1636,10 @@
       <c r="B49" s="16"/>
       <c r="C49" s="17"/>
       <c r="D49" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G49" s="14" t="n">
         <v>44</v>
@@ -1638,10 +1657,10 @@
       <c r="B50" s="16"/>
       <c r="C50" s="17"/>
       <c r="D50" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G50" s="14" t="n">
         <v>45</v>
@@ -1659,10 +1678,10 @@
       <c r="B51" s="20"/>
       <c r="C51" s="21"/>
       <c r="D51" s="20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G51" s="23" t="n">
         <v>46</v>

</xml_diff>

<commit_message>
Minor mod to pin layout
</commit_message>
<xml_diff>
--- a/hardware/pins.xlsx
+++ b/hardware/pins.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
   <si>
     <t xml:space="preserve">All pins are 3.3V logic</t>
   </si>
@@ -244,7 +244,13 @@
     <t xml:space="preserve">LCD Framer</t>
   </si>
   <si>
+    <t xml:space="preserve">GPIO (fake cs1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">gpio3[19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD760x #2</t>
   </si>
   <si>
     <t xml:space="preserve">gpio2[24]</t>
@@ -343,6 +349,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -364,12 +371,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,7 +490,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,17 +594,17 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,6 +688,7 @@
       <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C6" s="0"/>
       <c r="E6" s="9"/>
       <c r="G6" s="14" t="n">
         <v>1</v>
@@ -696,6 +706,7 @@
       <c r="B7" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="0"/>
       <c r="E7" s="9"/>
       <c r="G7" s="14" t="n">
         <v>2</v>
@@ -844,6 +855,7 @@
       <c r="A14" s="14" t="n">
         <v>9</v>
       </c>
+      <c r="C14" s="0"/>
       <c r="D14" s="0" t="s">
         <v>23</v>
       </c>
@@ -936,6 +948,7 @@
       <c r="A18" s="14" t="n">
         <v>13</v>
       </c>
+      <c r="C18" s="0"/>
       <c r="D18" s="0" t="s">
         <v>34</v>
       </c>
@@ -1090,6 +1103,7 @@
       <c r="A24" s="14" t="n">
         <v>19</v>
       </c>
+      <c r="C24" s="0"/>
       <c r="D24" s="0" t="s">
         <v>54</v>
       </c>
@@ -1247,6 +1261,7 @@
       <c r="A31" s="14" t="n">
         <v>26</v>
       </c>
+      <c r="C31" s="0"/>
       <c r="D31" s="0" t="s">
         <v>70</v>
       </c>
@@ -1275,11 +1290,16 @@
       <c r="G32" s="14" t="n">
         <v>27</v>
       </c>
+      <c r="H32" s="0" t="s">
+        <v>74</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="K32" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="n">
@@ -1288,7 +1308,7 @@
       <c r="B33" s="16"/>
       <c r="C33" s="17"/>
       <c r="D33" s="16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>73</v>
@@ -1297,16 +1317,16 @@
         <v>28</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,7 +1336,7 @@
       <c r="B34" s="16"/>
       <c r="C34" s="17"/>
       <c r="D34" s="16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>73</v>
@@ -1325,13 +1345,13 @@
         <v>29</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I34" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K34" s="9"/>
     </row>
@@ -1342,7 +1362,7 @@
       <c r="B35" s="16"/>
       <c r="C35" s="17"/>
       <c r="D35" s="16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>73</v>
@@ -1351,16 +1371,16 @@
         <v>30</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I35" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,7 +1390,7 @@
       <c r="B36" s="16"/>
       <c r="C36" s="17"/>
       <c r="D36" s="16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>73</v>
@@ -1379,16 +1399,16 @@
         <v>31</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I36" s="1" t="n">
         <v>3</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,7 +1418,7 @@
       <c r="B37" s="16"/>
       <c r="C37" s="17"/>
       <c r="D37" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>73</v>
@@ -1416,7 +1436,7 @@
       <c r="B38" s="16"/>
       <c r="C38" s="17"/>
       <c r="D38" s="16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>73</v>
@@ -1434,7 +1454,7 @@
       <c r="B39" s="16"/>
       <c r="C39" s="17"/>
       <c r="D39" s="16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>73</v>
@@ -1452,7 +1472,7 @@
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
       <c r="D40" s="16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>73</v>
@@ -1470,7 +1490,7 @@
       <c r="B41" s="16"/>
       <c r="C41" s="17"/>
       <c r="D41" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>73</v>
@@ -1488,7 +1508,7 @@
       <c r="B42" s="16"/>
       <c r="C42" s="17"/>
       <c r="D42" s="16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>73</v>
@@ -1506,7 +1526,7 @@
       <c r="B43" s="16"/>
       <c r="C43" s="17"/>
       <c r="D43" s="16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>73</v>
@@ -1524,7 +1544,7 @@
       <c r="B44" s="16"/>
       <c r="C44" s="17"/>
       <c r="D44" s="16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E44" s="18" t="s">
         <v>73</v>
@@ -1542,7 +1562,7 @@
       <c r="B45" s="16"/>
       <c r="C45" s="17"/>
       <c r="D45" s="16" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>73</v>
@@ -1560,7 +1580,7 @@
       <c r="B46" s="16"/>
       <c r="C46" s="17"/>
       <c r="D46" s="16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>73</v>
@@ -1578,7 +1598,7 @@
       <c r="B47" s="16"/>
       <c r="C47" s="17"/>
       <c r="D47" s="16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>73</v>
@@ -1596,7 +1616,7 @@
       <c r="B48" s="16"/>
       <c r="C48" s="17"/>
       <c r="D48" s="16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E48" s="18" t="s">
         <v>73</v>
@@ -1617,7 +1637,7 @@
       <c r="B49" s="16"/>
       <c r="C49" s="17"/>
       <c r="D49" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>73</v>
@@ -1638,7 +1658,7 @@
       <c r="B50" s="16"/>
       <c r="C50" s="17"/>
       <c r="D50" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>73</v>
@@ -1659,7 +1679,7 @@
       <c r="B51" s="20"/>
       <c r="C51" s="21"/>
       <c r="D51" s="20" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E51" s="22" t="s">
         <v>73</v>

</xml_diff>